<commit_message>
aktuelle version von manu
</commit_message>
<xml_diff>
--- a/Projektorganisation/Plannung_BA_bicycleComputer.xlsx
+++ b/Projektorganisation/Plannung_BA_bicycleComputer.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheKing\Documents\GitHub\ba_bicycle_comp\Projektorganisation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23250" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="43">
   <si>
     <t xml:space="preserve">Nr. </t>
   </si>
@@ -129,22 +134,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Inbetriebnahme Prototyp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>- Hardware-Spezifikation erstellen
-- Prinzip verstehen</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Hardware Layout erstellen
 </t>
     </r>
@@ -208,12 +197,43 @@
     <t xml:space="preserve">2. Meilenstein: Kommunikation 
 </t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E-Management überarbeiten
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- BLE für ca. 10km/h auslegen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Inbetriebnahme Prototyp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Prinzip verstehen
+- Prototyp ausmessen</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -809,24 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -853,18 +855,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -877,18 +867,49 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -913,9 +934,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -953,9 +974,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -987,9 +1008,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,9 +1060,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1196,48 +1253,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DO29"/>
+  <dimension ref="A1:DO30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="106" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" customWidth="1"/>
+    <col min="6" max="106" width="2.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" ht="41.25">
+    <row r="1" spans="1:106" ht="39" x14ac:dyDescent="0.9">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:106" s="2" customFormat="1" ht="14.25"/>
-    <row r="3" spans="1:106" s="2" customFormat="1" ht="23.25">
+    <row r="2" spans="1:106" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:106" s="2" customFormat="1" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:106" s="2" customFormat="1" ht="14.25"/>
-    <row r="5" spans="1:106" s="2" customFormat="1">
+    <row r="4" spans="1:106" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:106" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:106" s="2" customFormat="1" ht="15.75" thickBot="1">
+    <row r="6" spans="1:106" s="2" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:106" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:106" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1245,143 +1302,143 @@
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="64">
         <v>0</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="38">
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="64">
         <v>1</v>
       </c>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="38">
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="64">
         <v>2</v>
       </c>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="43">
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="67">
         <v>3</v>
       </c>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="43">
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67">
         <v>4</v>
       </c>
-      <c r="AE7" s="43"/>
-      <c r="AF7" s="43"/>
-      <c r="AG7" s="43"/>
-      <c r="AH7" s="43"/>
-      <c r="AI7" s="43"/>
-      <c r="AJ7" s="43">
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67">
         <v>5</v>
       </c>
-      <c r="AK7" s="43"/>
-      <c r="AL7" s="43"/>
-      <c r="AM7" s="43"/>
-      <c r="AN7" s="43"/>
-      <c r="AO7" s="43"/>
-      <c r="AP7" s="43">
+      <c r="AK7" s="67"/>
+      <c r="AL7" s="67"/>
+      <c r="AM7" s="67"/>
+      <c r="AN7" s="67"/>
+      <c r="AO7" s="67"/>
+      <c r="AP7" s="67">
         <v>6</v>
       </c>
-      <c r="AQ7" s="43"/>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="43"/>
-      <c r="AT7" s="43"/>
-      <c r="AU7" s="43"/>
-      <c r="AV7" s="43">
+      <c r="AQ7" s="67"/>
+      <c r="AR7" s="67"/>
+      <c r="AS7" s="67"/>
+      <c r="AT7" s="67"/>
+      <c r="AU7" s="67"/>
+      <c r="AV7" s="67">
         <v>7</v>
       </c>
-      <c r="AW7" s="43"/>
-      <c r="AX7" s="43"/>
-      <c r="AY7" s="43"/>
-      <c r="AZ7" s="43"/>
-      <c r="BA7" s="43"/>
-      <c r="BB7" s="43">
+      <c r="AW7" s="67"/>
+      <c r="AX7" s="67"/>
+      <c r="AY7" s="67"/>
+      <c r="AZ7" s="67"/>
+      <c r="BA7" s="67"/>
+      <c r="BB7" s="67">
         <v>8</v>
       </c>
-      <c r="BC7" s="43"/>
-      <c r="BD7" s="43"/>
-      <c r="BE7" s="43"/>
-      <c r="BF7" s="43"/>
-      <c r="BG7" s="43"/>
-      <c r="BH7" s="43">
+      <c r="BC7" s="67"/>
+      <c r="BD7" s="67"/>
+      <c r="BE7" s="67"/>
+      <c r="BF7" s="67"/>
+      <c r="BG7" s="67"/>
+      <c r="BH7" s="67">
         <v>9</v>
       </c>
-      <c r="BI7" s="43"/>
-      <c r="BJ7" s="43"/>
-      <c r="BK7" s="43"/>
-      <c r="BL7" s="43"/>
-      <c r="BM7" s="43"/>
-      <c r="BN7" s="43">
+      <c r="BI7" s="67"/>
+      <c r="BJ7" s="67"/>
+      <c r="BK7" s="67"/>
+      <c r="BL7" s="67"/>
+      <c r="BM7" s="67"/>
+      <c r="BN7" s="67">
         <v>10</v>
       </c>
-      <c r="BO7" s="43"/>
-      <c r="BP7" s="43"/>
-      <c r="BQ7" s="43"/>
-      <c r="BR7" s="43"/>
-      <c r="BS7" s="43"/>
-      <c r="BT7" s="43">
+      <c r="BO7" s="67"/>
+      <c r="BP7" s="67"/>
+      <c r="BQ7" s="67"/>
+      <c r="BR7" s="67"/>
+      <c r="BS7" s="67"/>
+      <c r="BT7" s="67">
         <v>11</v>
       </c>
-      <c r="BU7" s="43"/>
-      <c r="BV7" s="43"/>
-      <c r="BW7" s="43"/>
-      <c r="BX7" s="43"/>
-      <c r="BY7" s="43"/>
-      <c r="BZ7" s="43">
+      <c r="BU7" s="67"/>
+      <c r="BV7" s="67"/>
+      <c r="BW7" s="67"/>
+      <c r="BX7" s="67"/>
+      <c r="BY7" s="67"/>
+      <c r="BZ7" s="67">
         <v>12</v>
       </c>
-      <c r="CA7" s="43"/>
-      <c r="CB7" s="43"/>
-      <c r="CC7" s="43"/>
-      <c r="CD7" s="43"/>
-      <c r="CE7" s="43"/>
-      <c r="CF7" s="38">
+      <c r="CA7" s="67"/>
+      <c r="CB7" s="67"/>
+      <c r="CC7" s="67"/>
+      <c r="CD7" s="67"/>
+      <c r="CE7" s="67"/>
+      <c r="CF7" s="64">
         <v>13</v>
       </c>
-      <c r="CG7" s="39"/>
-      <c r="CH7" s="39"/>
-      <c r="CI7" s="39"/>
-      <c r="CJ7" s="39"/>
-      <c r="CK7" s="40"/>
-      <c r="CL7" s="38">
+      <c r="CG7" s="65"/>
+      <c r="CH7" s="65"/>
+      <c r="CI7" s="65"/>
+      <c r="CJ7" s="65"/>
+      <c r="CK7" s="66"/>
+      <c r="CL7" s="64">
         <v>13</v>
       </c>
-      <c r="CM7" s="39"/>
-      <c r="CN7" s="39"/>
-      <c r="CO7" s="39"/>
-      <c r="CP7" s="39"/>
-      <c r="CQ7" s="40"/>
-      <c r="CR7" s="38">
+      <c r="CM7" s="65"/>
+      <c r="CN7" s="65"/>
+      <c r="CO7" s="65"/>
+      <c r="CP7" s="65"/>
+      <c r="CQ7" s="66"/>
+      <c r="CR7" s="64">
         <v>13</v>
       </c>
-      <c r="CS7" s="39"/>
-      <c r="CT7" s="39"/>
-      <c r="CU7" s="39"/>
-      <c r="CV7" s="39"/>
-      <c r="CW7" s="40"/>
-      <c r="CX7" s="43">
+      <c r="CS7" s="65"/>
+      <c r="CT7" s="65"/>
+      <c r="CU7" s="65"/>
+      <c r="CV7" s="65"/>
+      <c r="CW7" s="66"/>
+      <c r="CX7" s="67">
         <v>14</v>
       </c>
-      <c r="CY7" s="43"/>
-      <c r="CZ7" s="43"/>
-      <c r="DA7" s="43"/>
-      <c r="DB7" s="43"/>
+      <c r="CY7" s="67"/>
+      <c r="CZ7" s="67"/>
+      <c r="DA7" s="67"/>
+      <c r="DB7" s="67"/>
     </row>
-    <row r="8" spans="1:106" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="8" spans="1:106" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1389,129 +1446,129 @@
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="38" t="s">
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="39"/>
-      <c r="AF8" s="39"/>
-      <c r="AG8" s="39"/>
-      <c r="AH8" s="39"/>
-      <c r="AI8" s="39"/>
-      <c r="AJ8" s="39"/>
-      <c r="AK8" s="39"/>
-      <c r="AL8" s="39"/>
-      <c r="AM8" s="39"/>
-      <c r="AN8" s="39"/>
-      <c r="AO8" s="39"/>
-      <c r="AP8" s="39"/>
-      <c r="AQ8" s="39"/>
-      <c r="AR8" s="39"/>
-      <c r="AS8" s="40"/>
-      <c r="AT8" s="38" t="s">
+      <c r="T8" s="65"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="65"/>
+      <c r="Y8" s="65"/>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="65"/>
+      <c r="AG8" s="65"/>
+      <c r="AH8" s="65"/>
+      <c r="AI8" s="65"/>
+      <c r="AJ8" s="65"/>
+      <c r="AK8" s="65"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="65"/>
+      <c r="AN8" s="65"/>
+      <c r="AO8" s="65"/>
+      <c r="AP8" s="65"/>
+      <c r="AQ8" s="65"/>
+      <c r="AR8" s="65"/>
+      <c r="AS8" s="66"/>
+      <c r="AT8" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AU8" s="39"/>
-      <c r="AV8" s="39"/>
-      <c r="AW8" s="39"/>
-      <c r="AX8" s="39"/>
-      <c r="AY8" s="39"/>
-      <c r="AZ8" s="39"/>
-      <c r="BA8" s="39"/>
-      <c r="BB8" s="39"/>
-      <c r="BC8" s="39"/>
-      <c r="BD8" s="39"/>
-      <c r="BE8" s="39"/>
-      <c r="BF8" s="39"/>
-      <c r="BG8" s="39"/>
-      <c r="BH8" s="39"/>
-      <c r="BI8" s="39"/>
-      <c r="BJ8" s="39"/>
-      <c r="BK8" s="39"/>
-      <c r="BL8" s="39"/>
-      <c r="BM8" s="39"/>
-      <c r="BN8" s="39"/>
-      <c r="BO8" s="39"/>
-      <c r="BP8" s="39"/>
-      <c r="BQ8" s="39"/>
-      <c r="BR8" s="39"/>
-      <c r="BS8" s="40"/>
-      <c r="BT8" s="38" t="s">
+      <c r="AU8" s="65"/>
+      <c r="AV8" s="65"/>
+      <c r="AW8" s="65"/>
+      <c r="AX8" s="65"/>
+      <c r="AY8" s="65"/>
+      <c r="AZ8" s="65"/>
+      <c r="BA8" s="65"/>
+      <c r="BB8" s="65"/>
+      <c r="BC8" s="65"/>
+      <c r="BD8" s="65"/>
+      <c r="BE8" s="65"/>
+      <c r="BF8" s="65"/>
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65"/>
+      <c r="BL8" s="65"/>
+      <c r="BM8" s="65"/>
+      <c r="BN8" s="65"/>
+      <c r="BO8" s="65"/>
+      <c r="BP8" s="65"/>
+      <c r="BQ8" s="65"/>
+      <c r="BR8" s="65"/>
+      <c r="BS8" s="66"/>
+      <c r="BT8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="BU8" s="39"/>
-      <c r="BV8" s="39"/>
-      <c r="BW8" s="39"/>
-      <c r="BX8" s="39"/>
-      <c r="BY8" s="39"/>
-      <c r="BZ8" s="39"/>
-      <c r="CA8" s="39"/>
-      <c r="CB8" s="39"/>
-      <c r="CC8" s="39"/>
-      <c r="CD8" s="39"/>
-      <c r="CE8" s="39"/>
-      <c r="CF8" s="39"/>
-      <c r="CG8" s="39"/>
-      <c r="CH8" s="39"/>
-      <c r="CI8" s="39"/>
-      <c r="CJ8" s="39"/>
-      <c r="CK8" s="39"/>
-      <c r="CL8" s="39"/>
-      <c r="CM8" s="39"/>
-      <c r="CN8" s="39"/>
-      <c r="CO8" s="39"/>
-      <c r="CP8" s="39"/>
-      <c r="CQ8" s="39"/>
-      <c r="CR8" s="39"/>
-      <c r="CS8" s="40"/>
-      <c r="CT8" s="38" t="s">
+      <c r="BU8" s="65"/>
+      <c r="BV8" s="65"/>
+      <c r="BW8" s="65"/>
+      <c r="BX8" s="65"/>
+      <c r="BY8" s="65"/>
+      <c r="BZ8" s="65"/>
+      <c r="CA8" s="65"/>
+      <c r="CB8" s="65"/>
+      <c r="CC8" s="65"/>
+      <c r="CD8" s="65"/>
+      <c r="CE8" s="65"/>
+      <c r="CF8" s="65"/>
+      <c r="CG8" s="65"/>
+      <c r="CH8" s="65"/>
+      <c r="CI8" s="65"/>
+      <c r="CJ8" s="65"/>
+      <c r="CK8" s="65"/>
+      <c r="CL8" s="65"/>
+      <c r="CM8" s="65"/>
+      <c r="CN8" s="65"/>
+      <c r="CO8" s="65"/>
+      <c r="CP8" s="65"/>
+      <c r="CQ8" s="65"/>
+      <c r="CR8" s="65"/>
+      <c r="CS8" s="66"/>
+      <c r="CT8" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="CU8" s="39"/>
-      <c r="CV8" s="39"/>
-      <c r="CW8" s="39"/>
-      <c r="CX8" s="39"/>
-      <c r="CY8" s="39"/>
-      <c r="CZ8" s="39"/>
-      <c r="DA8" s="39"/>
-      <c r="DB8" s="40"/>
+      <c r="CU8" s="65"/>
+      <c r="CV8" s="65"/>
+      <c r="CW8" s="65"/>
+      <c r="CX8" s="65"/>
+      <c r="CY8" s="65"/>
+      <c r="CZ8" s="65"/>
+      <c r="DA8" s="65"/>
+      <c r="DB8" s="66"/>
     </row>
-    <row r="9" spans="1:106" s="2" customFormat="1" thickBot="1">
+    <row r="9" spans="1:106" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="49" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1821,20 +1878,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:106" s="2" customFormat="1" thickBot="1">
+    <row r="10" spans="1:106" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="50">
         <v>42415</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="51">
         <v>42417</v>
       </c>
-      <c r="E10" s="52"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="13"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -1937,12 +1994,12 @@
       <c r="DA10" s="23"/>
       <c r="DB10" s="15"/>
     </row>
-    <row r="11" spans="1:106" s="2" customFormat="1" ht="36" thickBot="1">
+    <row r="11" spans="1:106" s="2" customFormat="1" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="B11" s="46" t="s">
-        <v>36</v>
+      <c r="B11" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="C11" s="21">
         <v>42417</v>
@@ -2053,19 +2110,15 @@
       <c r="DA11" s="25"/>
       <c r="DB11" s="16"/>
     </row>
-    <row r="12" spans="1:106" s="2" customFormat="1" ht="24.75" thickBot="1">
+    <row r="12" spans="1:106" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="21">
-        <v>42426</v>
-      </c>
-      <c r="D12" s="22">
-        <v>42439</v>
-      </c>
+      <c r="B12" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="9"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
@@ -2083,12 +2136,12 @@
       <c r="S12" s="30"/>
       <c r="T12" s="30"/>
       <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="30"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
       <c r="AB12" s="25"/>
       <c r="AC12" s="25"/>
       <c r="AD12" s="25"/>
@@ -2169,242 +2222,242 @@
       <c r="DA12" s="25"/>
       <c r="DB12" s="16"/>
     </row>
-    <row r="13" spans="1:106" s="2" customFormat="1" ht="24.75" thickBot="1">
-      <c r="A13" s="64">
+    <row r="13" spans="1:106" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="66">
+      <c r="B13" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="21">
+        <v>42426</v>
+      </c>
+      <c r="D13" s="22">
         <v>42439</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70"/>
-      <c r="S13" s="70"/>
-      <c r="T13" s="70"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="71"/>
-      <c r="W13" s="70"/>
-      <c r="X13" s="70"/>
-      <c r="Y13" s="70"/>
-      <c r="Z13" s="70"/>
-      <c r="AA13" s="36"/>
-      <c r="AB13" s="70"/>
-      <c r="AC13" s="70"/>
-      <c r="AD13" s="70"/>
-      <c r="AE13" s="70"/>
-      <c r="AF13" s="70"/>
-      <c r="AG13" s="70"/>
-      <c r="AH13" s="70"/>
-      <c r="AI13" s="70"/>
-      <c r="AJ13" s="70"/>
-      <c r="AK13" s="70"/>
-      <c r="AL13" s="70"/>
-      <c r="AM13" s="70"/>
-      <c r="AN13" s="70"/>
-      <c r="AO13" s="70"/>
-      <c r="AP13" s="70"/>
-      <c r="AQ13" s="70"/>
-      <c r="AR13" s="70"/>
-      <c r="AS13" s="70"/>
-      <c r="AT13" s="70"/>
-      <c r="AU13" s="70"/>
-      <c r="AV13" s="70"/>
-      <c r="AW13" s="70"/>
-      <c r="AX13" s="70"/>
-      <c r="AY13" s="70"/>
-      <c r="AZ13" s="70"/>
-      <c r="BA13" s="70"/>
-      <c r="BB13" s="70"/>
-      <c r="BC13" s="70"/>
-      <c r="BD13" s="70"/>
-      <c r="BE13" s="70"/>
-      <c r="BF13" s="70"/>
-      <c r="BG13" s="70"/>
-      <c r="BH13" s="70"/>
-      <c r="BI13" s="70"/>
-      <c r="BJ13" s="70"/>
-      <c r="BK13" s="70"/>
-      <c r="BL13" s="70"/>
-      <c r="BM13" s="70"/>
-      <c r="BN13" s="70"/>
-      <c r="BO13" s="70"/>
-      <c r="BP13" s="70"/>
-      <c r="BQ13" s="70"/>
-      <c r="BR13" s="70"/>
-      <c r="BS13" s="70"/>
-      <c r="BT13" s="70"/>
-      <c r="BU13" s="70"/>
-      <c r="BV13" s="70"/>
-      <c r="BW13" s="70"/>
-      <c r="BX13" s="70"/>
-      <c r="BY13" s="70"/>
-      <c r="BZ13" s="70"/>
-      <c r="CA13" s="70"/>
-      <c r="CB13" s="70"/>
-      <c r="CC13" s="70"/>
-      <c r="CD13" s="70"/>
-      <c r="CE13" s="70"/>
-      <c r="CF13" s="70"/>
-      <c r="CG13" s="70"/>
-      <c r="CH13" s="70"/>
-      <c r="CI13" s="70"/>
-      <c r="CJ13" s="70"/>
-      <c r="CK13" s="70"/>
-      <c r="CL13" s="70"/>
-      <c r="CM13" s="70"/>
-      <c r="CN13" s="70"/>
-      <c r="CO13" s="70"/>
-      <c r="CP13" s="70"/>
-      <c r="CQ13" s="70"/>
-      <c r="CR13" s="70"/>
-      <c r="CS13" s="70"/>
-      <c r="CT13" s="70"/>
-      <c r="CU13" s="70"/>
-      <c r="CV13" s="70"/>
-      <c r="CW13" s="70"/>
-      <c r="CX13" s="70"/>
-      <c r="CY13" s="70"/>
-      <c r="CZ13" s="70"/>
-      <c r="DA13" s="70"/>
-      <c r="DB13" s="72"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="25"/>
+      <c r="AJ13" s="25"/>
+      <c r="AK13" s="25"/>
+      <c r="AL13" s="25"/>
+      <c r="AM13" s="25"/>
+      <c r="AN13" s="25"/>
+      <c r="AO13" s="25"/>
+      <c r="AP13" s="25"/>
+      <c r="AQ13" s="25"/>
+      <c r="AR13" s="25"/>
+      <c r="AS13" s="25"/>
+      <c r="AT13" s="25"/>
+      <c r="AU13" s="25"/>
+      <c r="AV13" s="25"/>
+      <c r="AW13" s="25"/>
+      <c r="AX13" s="25"/>
+      <c r="AY13" s="25"/>
+      <c r="AZ13" s="25"/>
+      <c r="BA13" s="25"/>
+      <c r="BB13" s="25"/>
+      <c r="BC13" s="25"/>
+      <c r="BD13" s="25"/>
+      <c r="BE13" s="25"/>
+      <c r="BF13" s="25"/>
+      <c r="BG13" s="25"/>
+      <c r="BH13" s="25"/>
+      <c r="BI13" s="25"/>
+      <c r="BJ13" s="25"/>
+      <c r="BK13" s="25"/>
+      <c r="BL13" s="25"/>
+      <c r="BM13" s="25"/>
+      <c r="BN13" s="25"/>
+      <c r="BO13" s="25"/>
+      <c r="BP13" s="25"/>
+      <c r="BQ13" s="25"/>
+      <c r="BR13" s="25"/>
+      <c r="BS13" s="25"/>
+      <c r="BT13" s="25"/>
+      <c r="BU13" s="25"/>
+      <c r="BV13" s="25"/>
+      <c r="BW13" s="25"/>
+      <c r="BX13" s="25"/>
+      <c r="BY13" s="25"/>
+      <c r="BZ13" s="25"/>
+      <c r="CA13" s="25"/>
+      <c r="CB13" s="25"/>
+      <c r="CC13" s="25"/>
+      <c r="CD13" s="25"/>
+      <c r="CE13" s="25"/>
+      <c r="CF13" s="25"/>
+      <c r="CG13" s="25"/>
+      <c r="CH13" s="25"/>
+      <c r="CI13" s="25"/>
+      <c r="CJ13" s="25"/>
+      <c r="CK13" s="25"/>
+      <c r="CL13" s="25"/>
+      <c r="CM13" s="25"/>
+      <c r="CN13" s="25"/>
+      <c r="CO13" s="25"/>
+      <c r="CP13" s="25"/>
+      <c r="CQ13" s="25"/>
+      <c r="CR13" s="25"/>
+      <c r="CS13" s="25"/>
+      <c r="CT13" s="25"/>
+      <c r="CU13" s="25"/>
+      <c r="CV13" s="25"/>
+      <c r="CW13" s="25"/>
+      <c r="CX13" s="25"/>
+      <c r="CY13" s="25"/>
+      <c r="CZ13" s="25"/>
+      <c r="DA13" s="25"/>
+      <c r="DB13" s="16"/>
     </row>
-    <row r="14" spans="1:106" s="2" customFormat="1" thickBot="1">
-      <c r="A14" s="8">
+    <row r="14" spans="1:106" s="2" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="54">
         <v>5</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="21">
+      <c r="B14" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="72">
         <v>42439</v>
       </c>
-      <c r="D14" s="22">
-        <v>42453</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="73"/>
-      <c r="AB14" s="73"/>
-      <c r="AC14" s="73"/>
-      <c r="AD14" s="73"/>
-      <c r="AE14" s="73"/>
-      <c r="AF14" s="73"/>
-      <c r="AG14" s="73"/>
-      <c r="AH14" s="73"/>
-      <c r="AI14" s="73"/>
-      <c r="AJ14" s="73"/>
-      <c r="AK14" s="73"/>
-      <c r="AL14" s="73"/>
-      <c r="AM14" s="73"/>
-      <c r="AN14" s="25"/>
-      <c r="AO14" s="25"/>
-      <c r="AP14" s="25"/>
-      <c r="AQ14" s="25"/>
-      <c r="AR14" s="25"/>
-      <c r="AS14" s="25"/>
-      <c r="AT14" s="25"/>
-      <c r="AU14" s="25"/>
-      <c r="AV14" s="25"/>
-      <c r="AW14" s="25"/>
-      <c r="AX14" s="25"/>
-      <c r="AY14" s="25"/>
-      <c r="AZ14" s="25"/>
-      <c r="BA14" s="25"/>
-      <c r="BB14" s="25"/>
-      <c r="BC14" s="25"/>
-      <c r="BD14" s="25"/>
-      <c r="BE14" s="25"/>
-      <c r="BF14" s="25"/>
-      <c r="BG14" s="25"/>
-      <c r="BH14" s="25"/>
-      <c r="BI14" s="25"/>
-      <c r="BJ14" s="25"/>
-      <c r="BK14" s="25"/>
-      <c r="BL14" s="25"/>
-      <c r="BM14" s="25"/>
-      <c r="BN14" s="25"/>
-      <c r="BO14" s="25"/>
-      <c r="BP14" s="25"/>
-      <c r="BQ14" s="25"/>
-      <c r="BR14" s="25"/>
-      <c r="BS14" s="25"/>
-      <c r="BT14" s="25"/>
-      <c r="BU14" s="25"/>
-      <c r="BV14" s="25"/>
-      <c r="BW14" s="25"/>
-      <c r="BX14" s="25"/>
-      <c r="BY14" s="25"/>
-      <c r="BZ14" s="25"/>
-      <c r="CA14" s="25"/>
-      <c r="CB14" s="25"/>
-      <c r="CC14" s="25"/>
-      <c r="CD14" s="25"/>
-      <c r="CE14" s="25"/>
-      <c r="CF14" s="25"/>
-      <c r="CG14" s="25"/>
-      <c r="CH14" s="25"/>
-      <c r="CI14" s="25"/>
-      <c r="CJ14" s="25"/>
-      <c r="CK14" s="25"/>
-      <c r="CL14" s="25"/>
-      <c r="CM14" s="25"/>
-      <c r="CN14" s="25"/>
-      <c r="CO14" s="25"/>
-      <c r="CP14" s="25"/>
-      <c r="CQ14" s="25"/>
-      <c r="CR14" s="25"/>
-      <c r="CS14" s="25"/>
-      <c r="CT14" s="25"/>
-      <c r="CU14" s="25"/>
-      <c r="CV14" s="25"/>
-      <c r="CW14" s="25"/>
-      <c r="CX14" s="25"/>
-      <c r="CY14" s="25"/>
-      <c r="CZ14" s="25"/>
-      <c r="DA14" s="25"/>
-      <c r="DB14" s="16"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="58"/>
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="58"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="58"/>
+      <c r="AM14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="58"/>
+      <c r="AR14" s="58"/>
+      <c r="AS14" s="58"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="58"/>
+      <c r="AV14" s="58"/>
+      <c r="AW14" s="58"/>
+      <c r="AX14" s="58"/>
+      <c r="AY14" s="58"/>
+      <c r="AZ14" s="58"/>
+      <c r="BA14" s="58"/>
+      <c r="BB14" s="58"/>
+      <c r="BC14" s="58"/>
+      <c r="BD14" s="58"/>
+      <c r="BE14" s="58"/>
+      <c r="BF14" s="58"/>
+      <c r="BG14" s="58"/>
+      <c r="BH14" s="58"/>
+      <c r="BI14" s="58"/>
+      <c r="BJ14" s="58"/>
+      <c r="BK14" s="58"/>
+      <c r="BL14" s="58"/>
+      <c r="BM14" s="58"/>
+      <c r="BN14" s="58"/>
+      <c r="BO14" s="58"/>
+      <c r="BP14" s="58"/>
+      <c r="BQ14" s="58"/>
+      <c r="BR14" s="58"/>
+      <c r="BS14" s="58"/>
+      <c r="BT14" s="58"/>
+      <c r="BU14" s="58"/>
+      <c r="BV14" s="58"/>
+      <c r="BW14" s="58"/>
+      <c r="BX14" s="58"/>
+      <c r="BY14" s="58"/>
+      <c r="BZ14" s="58"/>
+      <c r="CA14" s="58"/>
+      <c r="CB14" s="58"/>
+      <c r="CC14" s="58"/>
+      <c r="CD14" s="58"/>
+      <c r="CE14" s="58"/>
+      <c r="CF14" s="58"/>
+      <c r="CG14" s="58"/>
+      <c r="CH14" s="58"/>
+      <c r="CI14" s="58"/>
+      <c r="CJ14" s="58"/>
+      <c r="CK14" s="58"/>
+      <c r="CL14" s="58"/>
+      <c r="CM14" s="58"/>
+      <c r="CN14" s="58"/>
+      <c r="CO14" s="58"/>
+      <c r="CP14" s="58"/>
+      <c r="CQ14" s="58"/>
+      <c r="CR14" s="58"/>
+      <c r="CS14" s="58"/>
+      <c r="CT14" s="58"/>
+      <c r="CU14" s="58"/>
+      <c r="CV14" s="58"/>
+      <c r="CW14" s="58"/>
+      <c r="CX14" s="58"/>
+      <c r="CY14" s="58"/>
+      <c r="CZ14" s="58"/>
+      <c r="DA14" s="58"/>
+      <c r="DB14" s="60"/>
     </row>
-    <row r="15" spans="1:106" s="2" customFormat="1" ht="36" thickBot="1">
+    <row r="15" spans="1:106" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>6</v>
       </c>
-      <c r="B15" s="46" t="s">
-        <v>39</v>
+      <c r="B15" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="21">
         <v>42439</v>
@@ -2428,29 +2481,29 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
+      <c r="U15" s="26"/>
       <c r="V15" s="25"/>
       <c r="W15" s="25"/>
       <c r="X15" s="25"/>
       <c r="Y15" s="25"/>
       <c r="Z15" s="25"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="30"/>
-      <c r="AE15" s="30"/>
-      <c r="AF15" s="30"/>
-      <c r="AG15" s="30"/>
-      <c r="AH15" s="25"/>
-      <c r="AI15" s="25"/>
-      <c r="AJ15" s="25"/>
-      <c r="AK15" s="25"/>
-      <c r="AL15" s="25"/>
-      <c r="AM15" s="25"/>
-      <c r="AN15" s="25"/>
-      <c r="AO15" s="25"/>
-      <c r="AP15" s="25"/>
-      <c r="AQ15" s="25"/>
+      <c r="AA15" s="74"/>
+      <c r="AB15" s="74"/>
+      <c r="AC15" s="74"/>
+      <c r="AD15" s="74"/>
+      <c r="AE15" s="74"/>
+      <c r="AF15" s="74"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
+      <c r="AK15" s="61"/>
+      <c r="AL15" s="61"/>
+      <c r="AM15" s="61"/>
+      <c r="AN15" s="61"/>
+      <c r="AO15" s="61"/>
+      <c r="AP15" s="61"/>
+      <c r="AQ15" s="61"/>
       <c r="AR15" s="25"/>
       <c r="AS15" s="25"/>
       <c r="AT15" s="25"/>
@@ -2515,12 +2568,12 @@
       <c r="DA15" s="25"/>
       <c r="DB15" s="16"/>
     </row>
-    <row r="16" spans="1:106" s="2" customFormat="1" ht="26.25" thickBot="1">
+    <row r="16" spans="1:106" s="2" customFormat="1" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>7</v>
       </c>
-      <c r="B16" s="47" t="s">
-        <v>32</v>
+      <c r="B16" s="40" t="s">
+        <v>38</v>
       </c>
       <c r="C16" s="21">
         <v>42439</v>
@@ -2557,12 +2610,12 @@
       <c r="AE16" s="30"/>
       <c r="AF16" s="30"/>
       <c r="AG16" s="30"/>
-      <c r="AH16" s="30"/>
-      <c r="AI16" s="30"/>
-      <c r="AJ16" s="30"/>
-      <c r="AK16" s="30"/>
-      <c r="AL16" s="30"/>
-      <c r="AM16" s="30"/>
+      <c r="AH16" s="25"/>
+      <c r="AI16" s="25"/>
+      <c r="AJ16" s="25"/>
+      <c r="AK16" s="25"/>
+      <c r="AL16" s="25"/>
+      <c r="AM16" s="25"/>
       <c r="AN16" s="25"/>
       <c r="AO16" s="25"/>
       <c r="AP16" s="25"/>
@@ -2631,20 +2684,20 @@
       <c r="DA16" s="25"/>
       <c r="DB16" s="16"/>
     </row>
-    <row r="17" spans="1:119" s="33" customFormat="1" ht="24.75" thickBot="1">
-      <c r="A17" s="31">
+    <row r="17" spans="1:119" s="2" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="34">
+      <c r="B17" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="21">
+        <v>42439</v>
+      </c>
+      <c r="D17" s="22">
         <v>42453</v>
       </c>
-      <c r="D17" s="35">
-        <v>42460</v>
-      </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="24"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -2666,25 +2719,25 @@
       <c r="X17" s="25"/>
       <c r="Y17" s="25"/>
       <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
-      <c r="AD17" s="25"/>
-      <c r="AE17" s="25"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
-      <c r="AH17" s="25"/>
-      <c r="AI17" s="25"/>
-      <c r="AJ17" s="25"/>
-      <c r="AK17" s="25"/>
-      <c r="AL17" s="25"/>
-      <c r="AM17" s="25"/>
-      <c r="AN17" s="30"/>
-      <c r="AO17" s="30"/>
-      <c r="AP17" s="30"/>
-      <c r="AQ17" s="30"/>
-      <c r="AR17" s="30"/>
-      <c r="AS17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
+      <c r="AQ17" s="25"/>
+      <c r="AR17" s="25"/>
+      <c r="AS17" s="25"/>
       <c r="AT17" s="25"/>
       <c r="AU17" s="25"/>
       <c r="AV17" s="25"/>
@@ -2745,20 +2798,22 @@
       <c r="CY17" s="25"/>
       <c r="CZ17" s="25"/>
       <c r="DA17" s="25"/>
-      <c r="DB17" s="32"/>
+      <c r="DB17" s="16"/>
     </row>
-    <row r="18" spans="1:119" s="33" customFormat="1" ht="26.25" thickBot="1">
+    <row r="18" spans="1:119" s="33" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>9</v>
       </c>
-      <c r="B18" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="60">
+      <c r="B18" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="34">
+        <v>42453</v>
+      </c>
+      <c r="D18" s="35">
         <v>42460</v>
       </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="53"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="24"/>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -2792,13 +2847,13 @@
       <c r="AJ18" s="25"/>
       <c r="AK18" s="25"/>
       <c r="AL18" s="25"/>
-      <c r="AM18" s="26"/>
-      <c r="AN18" s="25"/>
-      <c r="AO18" s="25"/>
-      <c r="AP18" s="25"/>
-      <c r="AQ18" s="25"/>
-      <c r="AR18" s="25"/>
-      <c r="AS18" s="36"/>
+      <c r="AM18" s="25"/>
+      <c r="AN18" s="30"/>
+      <c r="AO18" s="30"/>
+      <c r="AP18" s="30"/>
+      <c r="AQ18" s="30"/>
+      <c r="AR18" s="30"/>
+      <c r="AS18" s="30"/>
       <c r="AT18" s="25"/>
       <c r="AU18" s="25"/>
       <c r="AV18" s="25"/>
@@ -2861,20 +2916,18 @@
       <c r="DA18" s="25"/>
       <c r="DB18" s="32"/>
     </row>
-    <row r="19" spans="1:119" s="33" customFormat="1" ht="26.25" thickBot="1">
+    <row r="19" spans="1:119" s="33" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>10</v>
       </c>
-      <c r="B19" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="34">
+      <c r="B19" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="68">
         <v>42460</v>
       </c>
-      <c r="D19" s="35">
-        <v>42443</v>
-      </c>
-      <c r="E19" s="53"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="24"/>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -2908,24 +2961,24 @@
       <c r="AJ19" s="25"/>
       <c r="AK19" s="25"/>
       <c r="AL19" s="25"/>
-      <c r="AM19" s="25"/>
+      <c r="AM19" s="26"/>
       <c r="AN19" s="25"/>
       <c r="AO19" s="25"/>
       <c r="AP19" s="25"/>
       <c r="AQ19" s="25"/>
       <c r="AR19" s="25"/>
-      <c r="AS19" s="30"/>
-      <c r="AT19" s="30"/>
-      <c r="AU19" s="30"/>
-      <c r="AV19" s="30"/>
-      <c r="AW19" s="30"/>
-      <c r="AX19" s="30"/>
-      <c r="AY19" s="30"/>
-      <c r="AZ19" s="30"/>
-      <c r="BA19" s="30"/>
-      <c r="BB19" s="30"/>
-      <c r="BC19" s="30"/>
-      <c r="BD19" s="30"/>
+      <c r="AS19" s="36"/>
+      <c r="AT19" s="25"/>
+      <c r="AU19" s="25"/>
+      <c r="AV19" s="25"/>
+      <c r="AW19" s="25"/>
+      <c r="AX19" s="25"/>
+      <c r="AY19" s="25"/>
+      <c r="AZ19" s="25"/>
+      <c r="BA19" s="25"/>
+      <c r="BB19" s="25"/>
+      <c r="BC19" s="25"/>
+      <c r="BD19" s="25"/>
       <c r="BE19" s="25"/>
       <c r="BF19" s="25"/>
       <c r="BG19" s="25"/>
@@ -2977,20 +3030,20 @@
       <c r="DA19" s="25"/>
       <c r="DB19" s="32"/>
     </row>
-    <row r="20" spans="1:119" s="33" customFormat="1" thickBot="1">
+    <row r="20" spans="1:119" s="33" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>11</v>
       </c>
-      <c r="B20" s="49" t="s">
-        <v>33</v>
+      <c r="B20" s="42" t="s">
+        <v>23</v>
       </c>
       <c r="C20" s="34">
         <v>42460</v>
       </c>
       <c r="D20" s="35">
-        <v>42481</v>
-      </c>
-      <c r="E20" s="53"/>
+        <v>42443</v>
+      </c>
+      <c r="E20" s="47"/>
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
@@ -3042,13 +3095,13 @@
       <c r="BB20" s="30"/>
       <c r="BC20" s="30"/>
       <c r="BD20" s="30"/>
-      <c r="BE20" s="30"/>
-      <c r="BF20" s="30"/>
-      <c r="BG20" s="30"/>
-      <c r="BH20" s="30"/>
-      <c r="BI20" s="30"/>
-      <c r="BJ20" s="30"/>
-      <c r="BK20" s="30"/>
+      <c r="BE20" s="25"/>
+      <c r="BF20" s="25"/>
+      <c r="BG20" s="25"/>
+      <c r="BH20" s="25"/>
+      <c r="BI20" s="25"/>
+      <c r="BJ20" s="25"/>
+      <c r="BK20" s="25"/>
       <c r="BL20" s="25"/>
       <c r="BM20" s="25"/>
       <c r="BN20" s="25"/>
@@ -3093,20 +3146,20 @@
       <c r="DA20" s="25"/>
       <c r="DB20" s="32"/>
     </row>
-    <row r="21" spans="1:119" s="33" customFormat="1" ht="26.25" thickBot="1">
+    <row r="21" spans="1:119" s="33" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>12</v>
       </c>
-      <c r="B21" s="48" t="s">
-        <v>24</v>
+      <c r="B21" s="43" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="34">
-        <v>44300</v>
+        <v>42460</v>
       </c>
       <c r="D21" s="35">
         <v>42481</v>
       </c>
-      <c r="E21" s="53"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="24"/>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -3146,18 +3199,18 @@
       <c r="AP21" s="25"/>
       <c r="AQ21" s="25"/>
       <c r="AR21" s="25"/>
-      <c r="AS21" s="25"/>
-      <c r="AT21" s="25"/>
-      <c r="AU21" s="25"/>
-      <c r="AV21" s="25"/>
-      <c r="AW21" s="25"/>
-      <c r="AX21" s="25"/>
-      <c r="AY21" s="25"/>
-      <c r="AZ21" s="25"/>
-      <c r="BA21" s="25"/>
-      <c r="BB21" s="25"/>
-      <c r="BC21" s="25"/>
-      <c r="BD21" s="25"/>
+      <c r="AS21" s="30"/>
+      <c r="AT21" s="30"/>
+      <c r="AU21" s="30"/>
+      <c r="AV21" s="30"/>
+      <c r="AW21" s="30"/>
+      <c r="AX21" s="30"/>
+      <c r="AY21" s="30"/>
+      <c r="AZ21" s="30"/>
+      <c r="BA21" s="30"/>
+      <c r="BB21" s="30"/>
+      <c r="BC21" s="30"/>
+      <c r="BD21" s="30"/>
       <c r="BE21" s="30"/>
       <c r="BF21" s="30"/>
       <c r="BG21" s="30"/>
@@ -3209,18 +3262,20 @@
       <c r="DA21" s="25"/>
       <c r="DB21" s="32"/>
     </row>
-    <row r="22" spans="1:119" s="33" customFormat="1" ht="39" thickBot="1">
+    <row r="22" spans="1:119" s="33" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="31">
         <v>13</v>
       </c>
-      <c r="B22" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="60">
+      <c r="B22" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="34">
+        <v>44300</v>
+      </c>
+      <c r="D22" s="35">
         <v>42481</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="53"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
@@ -3272,13 +3327,13 @@
       <c r="BB22" s="25"/>
       <c r="BC22" s="25"/>
       <c r="BD22" s="25"/>
-      <c r="BE22" s="25"/>
-      <c r="BF22" s="25"/>
-      <c r="BG22" s="25"/>
-      <c r="BH22" s="25"/>
-      <c r="BI22" s="25"/>
-      <c r="BJ22" s="25"/>
-      <c r="BK22" s="36"/>
+      <c r="BE22" s="30"/>
+      <c r="BF22" s="30"/>
+      <c r="BG22" s="30"/>
+      <c r="BH22" s="30"/>
+      <c r="BI22" s="30"/>
+      <c r="BJ22" s="30"/>
+      <c r="BK22" s="30"/>
       <c r="BL22" s="25"/>
       <c r="BM22" s="25"/>
       <c r="BN22" s="25"/>
@@ -3323,20 +3378,18 @@
       <c r="DA22" s="25"/>
       <c r="DB22" s="32"/>
     </row>
-    <row r="23" spans="1:119" s="33" customFormat="1" thickBot="1">
+    <row r="23" spans="1:119" s="33" customFormat="1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31">
         <v>14</v>
       </c>
-      <c r="B23" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="62">
+      <c r="B23" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="68">
         <v>42481</v>
       </c>
-      <c r="D23" s="63">
-        <v>42509</v>
-      </c>
-      <c r="E23" s="53"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="24"/>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
@@ -3394,37 +3447,37 @@
       <c r="BH23" s="25"/>
       <c r="BI23" s="25"/>
       <c r="BJ23" s="25"/>
-      <c r="BK23" s="30"/>
-      <c r="BL23" s="30"/>
-      <c r="BM23" s="30"/>
-      <c r="BN23" s="30"/>
-      <c r="BO23" s="30"/>
-      <c r="BP23" s="30"/>
-      <c r="BQ23" s="30"/>
-      <c r="BR23" s="30"/>
-      <c r="BS23" s="30"/>
-      <c r="BT23" s="30"/>
-      <c r="BU23" s="30"/>
-      <c r="BV23" s="30"/>
-      <c r="BW23" s="30"/>
-      <c r="BX23" s="30"/>
-      <c r="BY23" s="30"/>
-      <c r="BZ23" s="30"/>
-      <c r="CA23" s="30"/>
-      <c r="CB23" s="30"/>
-      <c r="CC23" s="30"/>
-      <c r="CD23" s="30"/>
-      <c r="CE23" s="30"/>
-      <c r="CF23" s="30"/>
-      <c r="CG23" s="30"/>
-      <c r="CH23" s="30"/>
-      <c r="CI23" s="30"/>
-      <c r="CJ23" s="30"/>
-      <c r="CK23" s="30"/>
-      <c r="CL23" s="30"/>
-      <c r="CM23" s="30"/>
-      <c r="CN23" s="30"/>
-      <c r="CO23" s="30"/>
+      <c r="BK23" s="36"/>
+      <c r="BL23" s="25"/>
+      <c r="BM23" s="25"/>
+      <c r="BN23" s="25"/>
+      <c r="BO23" s="25"/>
+      <c r="BP23" s="25"/>
+      <c r="BQ23" s="25"/>
+      <c r="BR23" s="25"/>
+      <c r="BS23" s="25"/>
+      <c r="BT23" s="25"/>
+      <c r="BU23" s="25"/>
+      <c r="BV23" s="25"/>
+      <c r="BW23" s="25"/>
+      <c r="BX23" s="25"/>
+      <c r="BY23" s="25"/>
+      <c r="BZ23" s="25"/>
+      <c r="CA23" s="25"/>
+      <c r="CB23" s="25"/>
+      <c r="CC23" s="25"/>
+      <c r="CD23" s="25"/>
+      <c r="CE23" s="25"/>
+      <c r="CF23" s="25"/>
+      <c r="CG23" s="25"/>
+      <c r="CH23" s="25"/>
+      <c r="CI23" s="25"/>
+      <c r="CJ23" s="25"/>
+      <c r="CK23" s="25"/>
+      <c r="CL23" s="25"/>
+      <c r="CM23" s="25"/>
+      <c r="CN23" s="25"/>
+      <c r="CO23" s="25"/>
       <c r="CP23" s="25"/>
       <c r="CQ23" s="25"/>
       <c r="CR23" s="25"/>
@@ -3439,18 +3492,20 @@
       <c r="DA23" s="25"/>
       <c r="DB23" s="32"/>
     </row>
-    <row r="24" spans="1:119" s="33" customFormat="1" ht="26.25" thickBot="1">
+    <row r="24" spans="1:119" s="33" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31">
         <v>15</v>
       </c>
-      <c r="B24" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="62">
+      <c r="B24" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="52">
+        <v>42481</v>
+      </c>
+      <c r="D24" s="53">
         <v>42509</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="53"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
@@ -3508,37 +3563,37 @@
       <c r="BH24" s="25"/>
       <c r="BI24" s="25"/>
       <c r="BJ24" s="25"/>
-      <c r="BK24" s="25"/>
-      <c r="BL24" s="25"/>
-      <c r="BM24" s="25"/>
-      <c r="BN24" s="25"/>
-      <c r="BO24" s="25"/>
-      <c r="BP24" s="25"/>
-      <c r="BQ24" s="25"/>
-      <c r="BR24" s="25"/>
-      <c r="BS24" s="25"/>
-      <c r="BT24" s="25"/>
-      <c r="BU24" s="25"/>
-      <c r="BV24" s="25"/>
-      <c r="BW24" s="25"/>
-      <c r="BX24" s="25"/>
-      <c r="BY24" s="25"/>
-      <c r="BZ24" s="25"/>
-      <c r="CA24" s="25"/>
-      <c r="CB24" s="25"/>
-      <c r="CC24" s="25"/>
-      <c r="CD24" s="25"/>
-      <c r="CE24" s="25"/>
-      <c r="CF24" s="25"/>
-      <c r="CG24" s="25"/>
-      <c r="CH24" s="25"/>
-      <c r="CI24" s="36"/>
-      <c r="CJ24" s="25"/>
-      <c r="CK24" s="25"/>
-      <c r="CL24" s="25"/>
-      <c r="CM24" s="25"/>
-      <c r="CN24" s="25"/>
-      <c r="CO24" s="25"/>
+      <c r="BK24" s="30"/>
+      <c r="BL24" s="30"/>
+      <c r="BM24" s="30"/>
+      <c r="BN24" s="30"/>
+      <c r="BO24" s="30"/>
+      <c r="BP24" s="30"/>
+      <c r="BQ24" s="30"/>
+      <c r="BR24" s="30"/>
+      <c r="BS24" s="30"/>
+      <c r="BT24" s="30"/>
+      <c r="BU24" s="30"/>
+      <c r="BV24" s="30"/>
+      <c r="BW24" s="30"/>
+      <c r="BX24" s="30"/>
+      <c r="BY24" s="30"/>
+      <c r="BZ24" s="30"/>
+      <c r="CA24" s="30"/>
+      <c r="CB24" s="30"/>
+      <c r="CC24" s="30"/>
+      <c r="CD24" s="30"/>
+      <c r="CE24" s="30"/>
+      <c r="CF24" s="30"/>
+      <c r="CG24" s="30"/>
+      <c r="CH24" s="30"/>
+      <c r="CI24" s="30"/>
+      <c r="CJ24" s="30"/>
+      <c r="CK24" s="30"/>
+      <c r="CL24" s="30"/>
+      <c r="CM24" s="30"/>
+      <c r="CN24" s="30"/>
+      <c r="CO24" s="30"/>
       <c r="CP24" s="25"/>
       <c r="CQ24" s="25"/>
       <c r="CR24" s="25"/>
@@ -3553,20 +3608,18 @@
       <c r="DA24" s="25"/>
       <c r="DB24" s="32"/>
     </row>
-    <row r="25" spans="1:119" s="33" customFormat="1" thickBot="1">
+    <row r="25" spans="1:119" s="33" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31">
         <v>16</v>
       </c>
-      <c r="B25" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="62">
+      <c r="B25" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="52">
         <v>42509</v>
       </c>
-      <c r="D25" s="63">
-        <v>42646</v>
-      </c>
-      <c r="E25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="24"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -3648,19 +3701,19 @@
       <c r="CF25" s="25"/>
       <c r="CG25" s="25"/>
       <c r="CH25" s="25"/>
-      <c r="CI25" s="30"/>
-      <c r="CJ25" s="30"/>
-      <c r="CK25" s="30"/>
-      <c r="CL25" s="30"/>
-      <c r="CM25" s="30"/>
-      <c r="CN25" s="30"/>
-      <c r="CO25" s="30"/>
-      <c r="CP25" s="30"/>
-      <c r="CQ25" s="30"/>
-      <c r="CR25" s="30"/>
-      <c r="CS25" s="30"/>
-      <c r="CT25" s="30"/>
-      <c r="CU25" s="30"/>
+      <c r="CI25" s="36"/>
+      <c r="CJ25" s="25"/>
+      <c r="CK25" s="25"/>
+      <c r="CL25" s="25"/>
+      <c r="CM25" s="25"/>
+      <c r="CN25" s="25"/>
+      <c r="CO25" s="25"/>
+      <c r="CP25" s="25"/>
+      <c r="CQ25" s="25"/>
+      <c r="CR25" s="25"/>
+      <c r="CS25" s="25"/>
+      <c r="CT25" s="25"/>
+      <c r="CU25" s="25"/>
       <c r="CV25" s="25"/>
       <c r="CW25" s="25"/>
       <c r="CX25" s="25"/>
@@ -3669,20 +3722,20 @@
       <c r="DA25" s="25"/>
       <c r="DB25" s="32"/>
     </row>
-    <row r="26" spans="1:119" s="33" customFormat="1" thickBot="1">
+    <row r="26" spans="1:119" s="33" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31">
         <v>17</v>
       </c>
-      <c r="B26" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="62">
+      <c r="B26" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="52">
+        <v>42509</v>
+      </c>
+      <c r="D26" s="53">
         <v>42646</v>
       </c>
-      <c r="D26" s="63">
-        <v>42650</v>
-      </c>
-      <c r="E26" s="53"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="24"/>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
@@ -3764,39 +3817,41 @@
       <c r="CF26" s="25"/>
       <c r="CG26" s="25"/>
       <c r="CH26" s="25"/>
-      <c r="CI26" s="25"/>
-      <c r="CJ26" s="25"/>
-      <c r="CK26" s="25"/>
-      <c r="CL26" s="25"/>
-      <c r="CM26" s="25"/>
-      <c r="CN26" s="25"/>
-      <c r="CO26" s="25"/>
-      <c r="CP26" s="25"/>
-      <c r="CQ26" s="25"/>
-      <c r="CR26" s="25"/>
-      <c r="CS26" s="25"/>
-      <c r="CT26" s="25"/>
-      <c r="CU26" s="25"/>
-      <c r="CV26" s="37"/>
-      <c r="CW26" s="37"/>
-      <c r="CX26" s="37"/>
-      <c r="CY26" s="37"/>
+      <c r="CI26" s="30"/>
+      <c r="CJ26" s="30"/>
+      <c r="CK26" s="30"/>
+      <c r="CL26" s="30"/>
+      <c r="CM26" s="30"/>
+      <c r="CN26" s="30"/>
+      <c r="CO26" s="30"/>
+      <c r="CP26" s="30"/>
+      <c r="CQ26" s="30"/>
+      <c r="CR26" s="30"/>
+      <c r="CS26" s="30"/>
+      <c r="CT26" s="30"/>
+      <c r="CU26" s="30"/>
+      <c r="CV26" s="25"/>
+      <c r="CW26" s="25"/>
+      <c r="CX26" s="25"/>
+      <c r="CY26" s="25"/>
       <c r="CZ26" s="25"/>
       <c r="DA26" s="25"/>
       <c r="DB26" s="32"/>
     </row>
-    <row r="27" spans="1:119" s="2" customFormat="1" thickBot="1">
-      <c r="A27" s="8">
+    <row r="27" spans="1:119" s="33" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31">
         <v>18</v>
       </c>
-      <c r="B27" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="52">
+        <v>42646</v>
+      </c>
+      <c r="D27" s="53">
+        <v>42650</v>
+      </c>
+      <c r="E27" s="47"/>
       <c r="F27" s="24"/>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
@@ -3891,25 +3946,25 @@
       <c r="CS27" s="25"/>
       <c r="CT27" s="25"/>
       <c r="CU27" s="25"/>
-      <c r="CV27" s="25"/>
-      <c r="CW27" s="25"/>
-      <c r="CX27" s="25"/>
-      <c r="CY27" s="25"/>
+      <c r="CV27" s="37"/>
+      <c r="CW27" s="37"/>
+      <c r="CX27" s="37"/>
+      <c r="CY27" s="37"/>
       <c r="CZ27" s="25"/>
       <c r="DA27" s="25"/>
-      <c r="DB27" s="16"/>
+      <c r="DB27" s="32"/>
     </row>
-    <row r="28" spans="1:119" s="2" customFormat="1" thickBot="1">
+    <row r="28" spans="1:119" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>19</v>
       </c>
-      <c r="B28" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="58">
-        <v>42531</v>
-      </c>
-      <c r="D28" s="59"/>
+      <c r="B28" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="71"/>
       <c r="E28" s="9"/>
       <c r="F28" s="24"/>
       <c r="G28" s="25"/>
@@ -4011,138 +4066,264 @@
       <c r="CY28" s="25"/>
       <c r="CZ28" s="25"/>
       <c r="DA28" s="25"/>
-      <c r="DB28" s="17"/>
+      <c r="DB28" s="16"/>
     </row>
-    <row r="29" spans="1:119" s="2" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A29" s="10">
+    <row r="29" spans="1:119" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
         <v>20</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="70">
+        <v>42531</v>
+      </c>
+      <c r="D29" s="71"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="25"/>
+      <c r="Y29" s="25"/>
+      <c r="Z29" s="25"/>
+      <c r="AA29" s="25"/>
+      <c r="AB29" s="25"/>
+      <c r="AC29" s="25"/>
+      <c r="AD29" s="25"/>
+      <c r="AE29" s="25"/>
+      <c r="AF29" s="25"/>
+      <c r="AG29" s="25"/>
+      <c r="AH29" s="25"/>
+      <c r="AI29" s="25"/>
+      <c r="AJ29" s="25"/>
+      <c r="AK29" s="25"/>
+      <c r="AL29" s="25"/>
+      <c r="AM29" s="25"/>
+      <c r="AN29" s="25"/>
+      <c r="AO29" s="25"/>
+      <c r="AP29" s="25"/>
+      <c r="AQ29" s="25"/>
+      <c r="AR29" s="25"/>
+      <c r="AS29" s="25"/>
+      <c r="AT29" s="25"/>
+      <c r="AU29" s="25"/>
+      <c r="AV29" s="25"/>
+      <c r="AW29" s="25"/>
+      <c r="AX29" s="25"/>
+      <c r="AY29" s="25"/>
+      <c r="AZ29" s="25"/>
+      <c r="BA29" s="25"/>
+      <c r="BB29" s="25"/>
+      <c r="BC29" s="25"/>
+      <c r="BD29" s="25"/>
+      <c r="BE29" s="25"/>
+      <c r="BF29" s="25"/>
+      <c r="BG29" s="25"/>
+      <c r="BH29" s="25"/>
+      <c r="BI29" s="25"/>
+      <c r="BJ29" s="25"/>
+      <c r="BK29" s="25"/>
+      <c r="BL29" s="25"/>
+      <c r="BM29" s="25"/>
+      <c r="BN29" s="25"/>
+      <c r="BO29" s="25"/>
+      <c r="BP29" s="25"/>
+      <c r="BQ29" s="25"/>
+      <c r="BR29" s="25"/>
+      <c r="BS29" s="25"/>
+      <c r="BT29" s="25"/>
+      <c r="BU29" s="25"/>
+      <c r="BV29" s="25"/>
+      <c r="BW29" s="25"/>
+      <c r="BX29" s="25"/>
+      <c r="BY29" s="25"/>
+      <c r="BZ29" s="25"/>
+      <c r="CA29" s="25"/>
+      <c r="CB29" s="25"/>
+      <c r="CC29" s="25"/>
+      <c r="CD29" s="25"/>
+      <c r="CE29" s="25"/>
+      <c r="CF29" s="25"/>
+      <c r="CG29" s="25"/>
+      <c r="CH29" s="25"/>
+      <c r="CI29" s="25"/>
+      <c r="CJ29" s="25"/>
+      <c r="CK29" s="25"/>
+      <c r="CL29" s="25"/>
+      <c r="CM29" s="25"/>
+      <c r="CN29" s="25"/>
+      <c r="CO29" s="25"/>
+      <c r="CP29" s="25"/>
+      <c r="CQ29" s="25"/>
+      <c r="CR29" s="25"/>
+      <c r="CS29" s="25"/>
+      <c r="CT29" s="25"/>
+      <c r="CU29" s="25"/>
+      <c r="CV29" s="25"/>
+      <c r="CW29" s="25"/>
+      <c r="CX29" s="25"/>
+      <c r="CY29" s="25"/>
+      <c r="CZ29" s="25"/>
+      <c r="DA29" s="25"/>
+      <c r="DB29" s="17"/>
+    </row>
+    <row r="30" spans="1:119" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="10">
+        <v>21</v>
+      </c>
+      <c r="B30" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C30" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="28"/>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="19"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="20"/>
-      <c r="AE29" s="28"/>
-      <c r="AF29" s="20"/>
-      <c r="AG29" s="19"/>
-      <c r="AH29" s="20"/>
-      <c r="AI29" s="20"/>
-      <c r="AJ29" s="20"/>
-      <c r="AK29" s="28"/>
-      <c r="AL29" s="20"/>
-      <c r="AM29" s="19"/>
-      <c r="AN29" s="20"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
-      <c r="AQ29" s="28"/>
-      <c r="AR29" s="20"/>
-      <c r="AS29" s="19"/>
-      <c r="AT29" s="20"/>
-      <c r="AU29" s="20"/>
-      <c r="AV29" s="20"/>
-      <c r="AW29" s="28"/>
-      <c r="AX29" s="20"/>
-      <c r="AY29" s="19"/>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="20"/>
-      <c r="BB29" s="20"/>
-      <c r="BC29" s="28"/>
-      <c r="BD29" s="20"/>
-      <c r="BE29" s="19"/>
-      <c r="BF29" s="20"/>
-      <c r="BG29" s="20"/>
-      <c r="BH29" s="20"/>
-      <c r="BI29" s="28"/>
-      <c r="BJ29" s="20"/>
-      <c r="BK29" s="19"/>
-      <c r="BL29" s="20"/>
-      <c r="BM29" s="20"/>
-      <c r="BN29" s="20"/>
-      <c r="BO29" s="28"/>
-      <c r="BP29" s="20"/>
-      <c r="BQ29" s="19"/>
-      <c r="BR29" s="20"/>
-      <c r="BS29" s="20"/>
-      <c r="BT29" s="20"/>
-      <c r="BU29" s="28"/>
-      <c r="BV29" s="20"/>
-      <c r="BW29" s="19"/>
-      <c r="BX29" s="20"/>
-      <c r="BY29" s="20"/>
-      <c r="BZ29" s="20"/>
-      <c r="CA29" s="28"/>
-      <c r="CB29" s="20"/>
-      <c r="CC29" s="19"/>
-      <c r="CD29" s="20"/>
-      <c r="CE29" s="20"/>
-      <c r="CF29" s="20"/>
-      <c r="CG29" s="28"/>
-      <c r="CH29" s="20"/>
-      <c r="CI29" s="19"/>
-      <c r="CJ29" s="20"/>
-      <c r="CK29" s="20"/>
-      <c r="CL29" s="20"/>
-      <c r="CM29" s="28"/>
-      <c r="CN29" s="20"/>
-      <c r="CO29" s="19"/>
-      <c r="CP29" s="20"/>
-      <c r="CQ29" s="20"/>
-      <c r="CR29" s="20"/>
-      <c r="CS29" s="28"/>
-      <c r="CT29" s="20"/>
-      <c r="CU29" s="19"/>
-      <c r="CV29" s="28"/>
-      <c r="CW29" s="20"/>
-      <c r="CX29" s="20"/>
-      <c r="CY29" s="28"/>
-      <c r="CZ29" s="20"/>
-      <c r="DA29" s="28"/>
-      <c r="DB29" s="44"/>
-      <c r="DC29"/>
-      <c r="DD29"/>
-      <c r="DE29"/>
-      <c r="DF29"/>
-      <c r="DG29"/>
-      <c r="DH29"/>
-      <c r="DI29"/>
-      <c r="DJ29"/>
-      <c r="DK29"/>
-      <c r="DL29"/>
-      <c r="DM29"/>
-      <c r="DN29"/>
-      <c r="DO29"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="20"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="20"/>
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="20"/>
+      <c r="AE30" s="28"/>
+      <c r="AF30" s="20"/>
+      <c r="AG30" s="19"/>
+      <c r="AH30" s="20"/>
+      <c r="AI30" s="20"/>
+      <c r="AJ30" s="20"/>
+      <c r="AK30" s="28"/>
+      <c r="AL30" s="20"/>
+      <c r="AM30" s="19"/>
+      <c r="AN30" s="20"/>
+      <c r="AO30" s="20"/>
+      <c r="AP30" s="20"/>
+      <c r="AQ30" s="28"/>
+      <c r="AR30" s="20"/>
+      <c r="AS30" s="19"/>
+      <c r="AT30" s="20"/>
+      <c r="AU30" s="20"/>
+      <c r="AV30" s="20"/>
+      <c r="AW30" s="28"/>
+      <c r="AX30" s="20"/>
+      <c r="AY30" s="19"/>
+      <c r="AZ30" s="20"/>
+      <c r="BA30" s="20"/>
+      <c r="BB30" s="20"/>
+      <c r="BC30" s="28"/>
+      <c r="BD30" s="20"/>
+      <c r="BE30" s="19"/>
+      <c r="BF30" s="20"/>
+      <c r="BG30" s="20"/>
+      <c r="BH30" s="20"/>
+      <c r="BI30" s="28"/>
+      <c r="BJ30" s="20"/>
+      <c r="BK30" s="19"/>
+      <c r="BL30" s="20"/>
+      <c r="BM30" s="20"/>
+      <c r="BN30" s="20"/>
+      <c r="BO30" s="28"/>
+      <c r="BP30" s="20"/>
+      <c r="BQ30" s="19"/>
+      <c r="BR30" s="20"/>
+      <c r="BS30" s="20"/>
+      <c r="BT30" s="20"/>
+      <c r="BU30" s="28"/>
+      <c r="BV30" s="20"/>
+      <c r="BW30" s="19"/>
+      <c r="BX30" s="20"/>
+      <c r="BY30" s="20"/>
+      <c r="BZ30" s="20"/>
+      <c r="CA30" s="28"/>
+      <c r="CB30" s="20"/>
+      <c r="CC30" s="19"/>
+      <c r="CD30" s="20"/>
+      <c r="CE30" s="20"/>
+      <c r="CF30" s="20"/>
+      <c r="CG30" s="28"/>
+      <c r="CH30" s="20"/>
+      <c r="CI30" s="19"/>
+      <c r="CJ30" s="20"/>
+      <c r="CK30" s="20"/>
+      <c r="CL30" s="20"/>
+      <c r="CM30" s="28"/>
+      <c r="CN30" s="20"/>
+      <c r="CO30" s="19"/>
+      <c r="CP30" s="20"/>
+      <c r="CQ30" s="20"/>
+      <c r="CR30" s="20"/>
+      <c r="CS30" s="28"/>
+      <c r="CT30" s="20"/>
+      <c r="CU30" s="19"/>
+      <c r="CV30" s="28"/>
+      <c r="CW30" s="20"/>
+      <c r="CX30" s="20"/>
+      <c r="CY30" s="28"/>
+      <c r="CZ30" s="20"/>
+      <c r="DA30" s="28"/>
+      <c r="DB30" s="38"/>
+      <c r="DC30"/>
+      <c r="DD30"/>
+      <c r="DE30"/>
+      <c r="DF30"/>
+      <c r="DG30"/>
+      <c r="DH30"/>
+      <c r="DI30"/>
+      <c r="DJ30"/>
+      <c r="DK30"/>
+      <c r="DL30"/>
+      <c r="DM30"/>
+      <c r="DN30"/>
+      <c r="DO30"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="CF7:CK7"/>
+    <mergeCell ref="CL7:CQ7"/>
+    <mergeCell ref="BT8:CS8"/>
+    <mergeCell ref="CT8:DB8"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="S8:AS8"/>
+    <mergeCell ref="AT8:BS8"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="F8:R8"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="CR7:CW7"/>
     <mergeCell ref="CX7:DB7"/>
     <mergeCell ref="AV7:BA7"/>
@@ -4154,22 +4335,10 @@
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="L7:Q7"/>
     <mergeCell ref="X7:AC7"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="AD7:AI7"/>
     <mergeCell ref="AJ7:AO7"/>
     <mergeCell ref="AP7:AU7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="S8:AS8"/>
-    <mergeCell ref="AT8:BS8"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="F8:R8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="CF7:CK7"/>
-    <mergeCell ref="CL7:CQ7"/>
-    <mergeCell ref="BT8:CS8"/>
-    <mergeCell ref="CT8:DB8"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="30" orientation="landscape" r:id="rId1"/>
@@ -4177,24 +4346,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PDF der Plannung erstellt
</commit_message>
<xml_diff>
--- a/Projektorganisation/Plannung_BA_bicycleComputer.xlsx
+++ b/Projektorganisation/Plannung_BA_bicycleComputer.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$DB$29</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -913,24 +916,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -939,9 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="11" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -951,23 +933,14 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -992,6 +965,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,7 +1346,7 @@
   <dimension ref="A1:DO29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:DB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,141 +1388,141 @@
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="73">
         <v>0</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="49">
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="73">
         <v>1</v>
       </c>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="49">
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="73">
         <v>2</v>
       </c>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="54">
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="75"/>
+      <c r="X7" s="76">
         <v>3</v>
       </c>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="54"/>
-      <c r="AC7" s="54"/>
-      <c r="AD7" s="54">
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
+      <c r="AD7" s="76">
         <v>4</v>
       </c>
-      <c r="AE7" s="54"/>
-      <c r="AF7" s="54"/>
-      <c r="AG7" s="54"/>
-      <c r="AH7" s="54"/>
-      <c r="AI7" s="54"/>
-      <c r="AJ7" s="54">
+      <c r="AE7" s="76"/>
+      <c r="AF7" s="76"/>
+      <c r="AG7" s="76"/>
+      <c r="AH7" s="76"/>
+      <c r="AI7" s="76"/>
+      <c r="AJ7" s="76">
         <v>5</v>
       </c>
-      <c r="AK7" s="54"/>
-      <c r="AL7" s="54"/>
-      <c r="AM7" s="54"/>
-      <c r="AN7" s="54"/>
-      <c r="AO7" s="54"/>
-      <c r="AP7" s="54">
+      <c r="AK7" s="76"/>
+      <c r="AL7" s="76"/>
+      <c r="AM7" s="76"/>
+      <c r="AN7" s="76"/>
+      <c r="AO7" s="76"/>
+      <c r="AP7" s="76">
         <v>6</v>
       </c>
-      <c r="AQ7" s="54"/>
-      <c r="AR7" s="54"/>
-      <c r="AS7" s="54"/>
-      <c r="AT7" s="54"/>
-      <c r="AU7" s="54"/>
-      <c r="AV7" s="54">
+      <c r="AQ7" s="76"/>
+      <c r="AR7" s="76"/>
+      <c r="AS7" s="76"/>
+      <c r="AT7" s="76"/>
+      <c r="AU7" s="76"/>
+      <c r="AV7" s="76">
         <v>7</v>
       </c>
-      <c r="AW7" s="54"/>
-      <c r="AX7" s="54"/>
-      <c r="AY7" s="54"/>
-      <c r="AZ7" s="54"/>
-      <c r="BA7" s="54"/>
-      <c r="BB7" s="54">
+      <c r="AW7" s="76"/>
+      <c r="AX7" s="76"/>
+      <c r="AY7" s="76"/>
+      <c r="AZ7" s="76"/>
+      <c r="BA7" s="76"/>
+      <c r="BB7" s="76">
         <v>8</v>
       </c>
-      <c r="BC7" s="54"/>
-      <c r="BD7" s="54"/>
-      <c r="BE7" s="54"/>
-      <c r="BF7" s="54"/>
-      <c r="BG7" s="54"/>
-      <c r="BH7" s="54">
+      <c r="BC7" s="76"/>
+      <c r="BD7" s="76"/>
+      <c r="BE7" s="76"/>
+      <c r="BF7" s="76"/>
+      <c r="BG7" s="76"/>
+      <c r="BH7" s="76">
         <v>9</v>
       </c>
-      <c r="BI7" s="54"/>
-      <c r="BJ7" s="54"/>
-      <c r="BK7" s="54"/>
-      <c r="BL7" s="54"/>
-      <c r="BM7" s="54"/>
-      <c r="BN7" s="54">
+      <c r="BI7" s="76"/>
+      <c r="BJ7" s="76"/>
+      <c r="BK7" s="76"/>
+      <c r="BL7" s="76"/>
+      <c r="BM7" s="76"/>
+      <c r="BN7" s="76">
         <v>10</v>
       </c>
-      <c r="BO7" s="54"/>
-      <c r="BP7" s="54"/>
-      <c r="BQ7" s="54"/>
-      <c r="BR7" s="54"/>
-      <c r="BS7" s="54"/>
-      <c r="BT7" s="54">
+      <c r="BO7" s="76"/>
+      <c r="BP7" s="76"/>
+      <c r="BQ7" s="76"/>
+      <c r="BR7" s="76"/>
+      <c r="BS7" s="76"/>
+      <c r="BT7" s="76">
         <v>11</v>
       </c>
-      <c r="BU7" s="54"/>
-      <c r="BV7" s="54"/>
-      <c r="BW7" s="54"/>
-      <c r="BX7" s="54"/>
-      <c r="BY7" s="54"/>
-      <c r="BZ7" s="54">
+      <c r="BU7" s="76"/>
+      <c r="BV7" s="76"/>
+      <c r="BW7" s="76"/>
+      <c r="BX7" s="76"/>
+      <c r="BY7" s="76"/>
+      <c r="BZ7" s="76">
         <v>12</v>
       </c>
-      <c r="CA7" s="54"/>
-      <c r="CB7" s="54"/>
-      <c r="CC7" s="54"/>
-      <c r="CD7" s="54"/>
-      <c r="CE7" s="54"/>
-      <c r="CF7" s="49">
+      <c r="CA7" s="76"/>
+      <c r="CB7" s="76"/>
+      <c r="CC7" s="76"/>
+      <c r="CD7" s="76"/>
+      <c r="CE7" s="76"/>
+      <c r="CF7" s="73">
         <v>13</v>
       </c>
-      <c r="CG7" s="50"/>
-      <c r="CH7" s="50"/>
-      <c r="CI7" s="50"/>
-      <c r="CJ7" s="50"/>
-      <c r="CK7" s="51"/>
-      <c r="CL7" s="49">
+      <c r="CG7" s="74"/>
+      <c r="CH7" s="74"/>
+      <c r="CI7" s="74"/>
+      <c r="CJ7" s="74"/>
+      <c r="CK7" s="75"/>
+      <c r="CL7" s="73">
         <v>13</v>
       </c>
-      <c r="CM7" s="50"/>
-      <c r="CN7" s="50"/>
-      <c r="CO7" s="50"/>
-      <c r="CP7" s="50"/>
-      <c r="CQ7" s="51"/>
-      <c r="CR7" s="49">
+      <c r="CM7" s="74"/>
+      <c r="CN7" s="74"/>
+      <c r="CO7" s="74"/>
+      <c r="CP7" s="74"/>
+      <c r="CQ7" s="75"/>
+      <c r="CR7" s="73">
         <v>13</v>
       </c>
-      <c r="CS7" s="50"/>
-      <c r="CT7" s="50"/>
-      <c r="CU7" s="50"/>
-      <c r="CV7" s="50"/>
-      <c r="CW7" s="51"/>
-      <c r="CX7" s="54">
+      <c r="CS7" s="74"/>
+      <c r="CT7" s="74"/>
+      <c r="CU7" s="74"/>
+      <c r="CV7" s="74"/>
+      <c r="CW7" s="75"/>
+      <c r="CX7" s="76">
         <v>14</v>
       </c>
-      <c r="CY7" s="54"/>
-      <c r="CZ7" s="54"/>
-      <c r="DA7" s="54"/>
-      <c r="DB7" s="54"/>
+      <c r="CY7" s="76"/>
+      <c r="CZ7" s="76"/>
+      <c r="DA7" s="76"/>
+      <c r="DB7" s="76"/>
     </row>
     <row r="8" spans="1:106" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
@@ -1529,117 +1532,117 @@
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="49" t="s">
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="50"/>
-      <c r="Z8" s="50"/>
-      <c r="AA8" s="50"/>
-      <c r="AB8" s="50"/>
-      <c r="AC8" s="50"/>
-      <c r="AD8" s="50"/>
-      <c r="AE8" s="50"/>
-      <c r="AF8" s="50"/>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="50"/>
-      <c r="AJ8" s="50"/>
-      <c r="AK8" s="50"/>
-      <c r="AL8" s="50"/>
-      <c r="AM8" s="50"/>
-      <c r="AN8" s="50"/>
-      <c r="AO8" s="50"/>
-      <c r="AP8" s="50"/>
-      <c r="AQ8" s="50"/>
-      <c r="AR8" s="50"/>
-      <c r="AS8" s="51"/>
-      <c r="AT8" s="49" t="s">
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="75"/>
+      <c r="AT8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="AU8" s="50"/>
-      <c r="AV8" s="50"/>
-      <c r="AW8" s="50"/>
-      <c r="AX8" s="50"/>
-      <c r="AY8" s="50"/>
-      <c r="AZ8" s="50"/>
-      <c r="BA8" s="50"/>
-      <c r="BB8" s="50"/>
-      <c r="BC8" s="50"/>
-      <c r="BD8" s="50"/>
-      <c r="BE8" s="50"/>
-      <c r="BF8" s="50"/>
-      <c r="BG8" s="50"/>
-      <c r="BH8" s="50"/>
-      <c r="BI8" s="50"/>
-      <c r="BJ8" s="50"/>
-      <c r="BK8" s="50"/>
-      <c r="BL8" s="50"/>
-      <c r="BM8" s="50"/>
-      <c r="BN8" s="50"/>
-      <c r="BO8" s="50"/>
-      <c r="BP8" s="50"/>
-      <c r="BQ8" s="50"/>
-      <c r="BR8" s="50"/>
-      <c r="BS8" s="51"/>
-      <c r="BT8" s="49" t="s">
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74"/>
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74"/>
+      <c r="BC8" s="74"/>
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74"/>
+      <c r="BG8" s="74"/>
+      <c r="BH8" s="74"/>
+      <c r="BI8" s="74"/>
+      <c r="BJ8" s="74"/>
+      <c r="BK8" s="74"/>
+      <c r="BL8" s="74"/>
+      <c r="BM8" s="74"/>
+      <c r="BN8" s="74"/>
+      <c r="BO8" s="74"/>
+      <c r="BP8" s="74"/>
+      <c r="BQ8" s="74"/>
+      <c r="BR8" s="74"/>
+      <c r="BS8" s="75"/>
+      <c r="BT8" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="BU8" s="50"/>
-      <c r="BV8" s="50"/>
-      <c r="BW8" s="50"/>
-      <c r="BX8" s="50"/>
-      <c r="BY8" s="50"/>
-      <c r="BZ8" s="50"/>
-      <c r="CA8" s="50"/>
-      <c r="CB8" s="50"/>
-      <c r="CC8" s="50"/>
-      <c r="CD8" s="50"/>
-      <c r="CE8" s="50"/>
-      <c r="CF8" s="50"/>
-      <c r="CG8" s="50"/>
-      <c r="CH8" s="50"/>
-      <c r="CI8" s="50"/>
-      <c r="CJ8" s="50"/>
-      <c r="CK8" s="50"/>
-      <c r="CL8" s="50"/>
-      <c r="CM8" s="50"/>
-      <c r="CN8" s="50"/>
-      <c r="CO8" s="50"/>
-      <c r="CP8" s="50"/>
-      <c r="CQ8" s="50"/>
-      <c r="CR8" s="50"/>
-      <c r="CS8" s="51"/>
-      <c r="CT8" s="49" t="s">
+      <c r="BU8" s="74"/>
+      <c r="BV8" s="74"/>
+      <c r="BW8" s="74"/>
+      <c r="BX8" s="74"/>
+      <c r="BY8" s="74"/>
+      <c r="BZ8" s="74"/>
+      <c r="CA8" s="74"/>
+      <c r="CB8" s="74"/>
+      <c r="CC8" s="74"/>
+      <c r="CD8" s="74"/>
+      <c r="CE8" s="74"/>
+      <c r="CF8" s="74"/>
+      <c r="CG8" s="74"/>
+      <c r="CH8" s="74"/>
+      <c r="CI8" s="74"/>
+      <c r="CJ8" s="74"/>
+      <c r="CK8" s="74"/>
+      <c r="CL8" s="74"/>
+      <c r="CM8" s="74"/>
+      <c r="CN8" s="74"/>
+      <c r="CO8" s="74"/>
+      <c r="CP8" s="74"/>
+      <c r="CQ8" s="74"/>
+      <c r="CR8" s="74"/>
+      <c r="CS8" s="75"/>
+      <c r="CT8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="CU8" s="50"/>
-      <c r="CV8" s="50"/>
-      <c r="CW8" s="50"/>
-      <c r="CX8" s="50"/>
-      <c r="CY8" s="50"/>
-      <c r="CZ8" s="50"/>
-      <c r="DA8" s="50"/>
-      <c r="DB8" s="51"/>
+      <c r="CU8" s="74"/>
+      <c r="CV8" s="74"/>
+      <c r="CW8" s="74"/>
+      <c r="CX8" s="74"/>
+      <c r="CY8" s="74"/>
+      <c r="CZ8" s="74"/>
+      <c r="DA8" s="74"/>
+      <c r="DB8" s="75"/>
     </row>
     <row r="9" spans="1:106" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -1965,10 +1968,10 @@
       <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="56">
         <v>42415</v>
       </c>
       <c r="D10" s="39">
@@ -2081,10 +2084,10 @@
       <c r="A11" s="8">
         <v>2</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="57">
         <v>42417</v>
       </c>
       <c r="D11" s="20">
@@ -2197,10 +2200,10 @@
       <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="57">
         <v>42426</v>
       </c>
       <c r="D12" s="20">
@@ -2313,10 +2316,10 @@
       <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="57">
         <v>42432</v>
       </c>
       <c r="D13" s="20">
@@ -2429,13 +2432,13 @@
       <c r="A14" s="41">
         <v>5</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="77">
         <v>42446</v>
       </c>
-      <c r="D14" s="52"/>
+      <c r="D14" s="78"/>
       <c r="E14" s="42"/>
       <c r="F14" s="43"/>
       <c r="G14" s="44"/>
@@ -2543,10 +2546,10 @@
       <c r="A15" s="8">
         <v>6</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="57">
         <v>42446</v>
       </c>
       <c r="D15" s="20">
@@ -2659,10 +2662,10 @@
       <c r="A16" s="8">
         <v>7</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="57">
         <v>42446</v>
       </c>
       <c r="D16" s="20">
@@ -2775,10 +2778,10 @@
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="64">
+      <c r="C17" s="57">
         <v>42446</v>
       </c>
       <c r="D17" s="20">
@@ -2888,20 +2891,20 @@
       <c r="DB17" s="16"/>
     </row>
     <row r="18" spans="1:119" s="31" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="58">
+      <c r="A18" s="52">
         <v>9</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="80">
+      <c r="C18" s="70">
         <v>42460</v>
       </c>
       <c r="D18" s="20">
         <v>42467</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="56"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="48"/>
       <c r="H18" s="48"/>
       <c r="I18" s="48"/>
@@ -3001,19 +3004,19 @@
       <c r="CY18" s="48"/>
       <c r="CZ18" s="48"/>
       <c r="DA18" s="48"/>
-      <c r="DB18" s="55"/>
+      <c r="DB18" s="49"/>
     </row>
     <row r="19" spans="1:119" s="31" customFormat="1" ht="24.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="41">
         <v>10</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="77">
         <v>42467</v>
       </c>
-      <c r="D19" s="52"/>
+      <c r="D19" s="78"/>
       <c r="E19" s="42"/>
       <c r="F19" s="43"/>
       <c r="G19" s="44"/>
@@ -3048,7 +3051,7 @@
       <c r="AJ19" s="44"/>
       <c r="AK19" s="44"/>
       <c r="AL19" s="44"/>
-      <c r="AM19" s="60"/>
+      <c r="AM19" s="54"/>
       <c r="AN19" s="44"/>
       <c r="AO19" s="44"/>
       <c r="AP19" s="44"/>
@@ -3121,10 +3124,10 @@
       <c r="A20" s="29">
         <v>11</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="66">
+      <c r="C20" s="58">
         <v>42467</v>
       </c>
       <c r="D20" s="32">
@@ -3237,10 +3240,10 @@
       <c r="A21" s="29">
         <v>12</v>
       </c>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="66">
+      <c r="C21" s="58">
         <v>42467</v>
       </c>
       <c r="D21" s="32">
@@ -3353,10 +3356,10 @@
       <c r="A22" s="29">
         <v>13</v>
       </c>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="66">
+      <c r="C22" s="58">
         <v>42474</v>
       </c>
       <c r="D22" s="32">
@@ -3469,13 +3472,13 @@
       <c r="A23" s="41">
         <v>14</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="65">
+      <c r="C23" s="77">
         <v>42481</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="42"/>
       <c r="F23" s="43"/>
       <c r="G23" s="44"/>
@@ -3583,10 +3586,10 @@
       <c r="A24" s="29">
         <v>15</v>
       </c>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="67">
+      <c r="C24" s="59">
         <v>42481</v>
       </c>
       <c r="D24" s="40">
@@ -3699,13 +3702,13 @@
       <c r="A25" s="41">
         <v>16</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="79">
         <v>42509</v>
       </c>
-      <c r="D25" s="61"/>
+      <c r="D25" s="80"/>
       <c r="E25" s="42"/>
       <c r="F25" s="43"/>
       <c r="G25" s="44"/>
@@ -3813,10 +3816,10 @@
       <c r="A26" s="29">
         <v>17</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="67">
+      <c r="C26" s="59">
         <v>42509</v>
       </c>
       <c r="D26" s="40">
@@ -3929,10 +3932,10 @@
       <c r="A27" s="29">
         <v>18</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="67">
+      <c r="C27" s="59">
         <v>42646</v>
       </c>
       <c r="D27" s="40">
@@ -4045,13 +4048,13 @@
       <c r="A28" s="41">
         <v>19</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="69">
+      <c r="C28" s="60">
         <v>42528</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="55">
         <v>42531</v>
       </c>
       <c r="E28" s="42"/>
@@ -4155,19 +4158,19 @@
       <c r="CY28" s="28"/>
       <c r="CZ28" s="28"/>
       <c r="DA28" s="28"/>
-      <c r="DB28" s="57"/>
+      <c r="DB28" s="51"/>
     </row>
     <row r="29" spans="1:119" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <v>20</v>
       </c>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="70" t="s">
+      <c r="C29" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="53"/>
+      <c r="D29" s="72"/>
       <c r="E29" s="11"/>
       <c r="F29" s="17"/>
       <c r="G29" s="26"/>
@@ -4286,6 +4289,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="CF7:CK7"/>
+    <mergeCell ref="CL7:CQ7"/>
+    <mergeCell ref="BT8:CS8"/>
+    <mergeCell ref="CT8:DB8"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="S8:AS8"/>
+    <mergeCell ref="AT8:BS8"/>
+    <mergeCell ref="R7:W7"/>
+    <mergeCell ref="F8:R8"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="CR7:CW7"/>
     <mergeCell ref="CX7:DB7"/>
@@ -4302,20 +4316,9 @@
     <mergeCell ref="AD7:AI7"/>
     <mergeCell ref="AJ7:AO7"/>
     <mergeCell ref="AP7:AU7"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="S8:AS8"/>
-    <mergeCell ref="AT8:BS8"/>
-    <mergeCell ref="R7:W7"/>
-    <mergeCell ref="F8:R8"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="CF7:CK7"/>
-    <mergeCell ref="CL7:CQ7"/>
-    <mergeCell ref="BT8:CS8"/>
-    <mergeCell ref="CT8:DB8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="28" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>